<commit_message>
Create logger for result
</commit_message>
<xml_diff>
--- a/out/production/RiddleHailing/Data.xlsx
+++ b/out/production/RiddleHailing/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RiddleHailing\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0011941E-6225-4B1B-ACA2-D53BE71C5887}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1596D79A-8C55-48B6-B0F3-313219E3F670}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver" sheetId="2" r:id="rId1"/>
@@ -449,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D6:D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,35 +598,71 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>14</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>14</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>4</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>14</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -762,7 +798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>

</xml_diff>